<commit_message>
fix typos and move ANO data to P:/
</commit_message>
<xml_diff>
--- a/indicators/NO_ALIE_001-004/metadata.xlsx
+++ b/indicators/NO_ALIE_001-004/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.grainger\Documents\Projects_in_development\ecRxiv\indicators\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R projects github\ecRxiv_aliens\indicators\NO_ALIE_001-004\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433C71A1-6EC0-4AA9-AEBA-19C7C8982435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A4677B-F40C-46E4-9AF6-E37E4C0571B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="18300" windowHeight="10420" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="209">
   <si>
     <t>indicatorID</t>
   </si>
@@ -602,9 +602,6 @@
   </si>
   <si>
     <t>Beta-versions are numbers incrementally with values below 0. Operational versions can be given the version numbers above 0. Use this terms similar as for software versioning,</t>
-  </si>
-  <si>
-    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/</t>
   </si>
   <si>
     <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/'INDICATOR-ID'</t>
@@ -694,6 +691,24 @@
   </si>
   <si>
     <t>A2 - Chemical State characteristics</t>
+  </si>
+  <si>
+    <t>NO_ALIE_001-004</t>
+  </si>
+  <si>
+    <t>area without alien plant species</t>
+  </si>
+  <si>
+    <t>T2 Temperate-boreal forests and woodlands biome, T3 Shrublands and shrubby woodlands biome, T6 Polar-alpine (cryogenic) biome</t>
+  </si>
+  <si>
+    <t>Töpper, J.</t>
+  </si>
+  <si>
+    <t>https://github.com/NINAnor/ecRxiv/tree/main/indicators/NO_ALIE_001-004</t>
+  </si>
+  <si>
+    <t>Scale - Aggregate</t>
   </si>
 </sst>
 </file>
@@ -1153,19 +1168,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78FF33B-C37D-487F-A5F6-37AB2202A4CF}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.88671875" customWidth="1"/>
-    <col min="2" max="2" width="47.88671875" customWidth="1"/>
-    <col min="3" max="3" width="106.44140625" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="47.90625" customWidth="1"/>
+    <col min="3" max="3" width="106.453125" customWidth="1"/>
     <col min="4" max="4" width="145" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1179,50 +1194,59 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>203</v>
+      </c>
       <c r="C2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>204</v>
+      </c>
       <c r="C3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1231,11 +1255,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1243,11 +1269,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>139</v>
       </c>
@@ -1255,7 +1283,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -1267,29 +1295,31 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>1901</v>
+        <v>2025</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>2025</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>164</v>
       </c>
@@ -1301,7 +1331,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>167</v>
       </c>
@@ -1315,7 +1345,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>168</v>
       </c>
@@ -1325,12 +1355,12 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>186</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>183</v>
@@ -1339,42 +1369,46 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>184</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="D16" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="D17" s="2" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -1434,19 +1468,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD06A-F7D1-4345-BCDF-E89F4B8A4AD5}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="60.6640625" customWidth="1"/>
+    <col min="1" max="1" width="60.6328125" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
     <col min="3" max="3" width="64" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1463,10 +1497,10 @@
         <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1483,12 +1517,12 @@
         <v>180</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
         <v>171</v>
@@ -1503,10 +1537,10 @@
         <v>181</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1523,7 +1557,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1537,7 +1571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1551,7 +1585,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -1565,7 +1599,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1579,7 +1613,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>177</v>
       </c>
@@ -1590,7 +1624,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>178</v>
       </c>
@@ -1601,7 +1635,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>147</v>
       </c>
@@ -1609,7 +1643,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>148</v>
       </c>
@@ -1617,7 +1651,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>149</v>
       </c>
@@ -1625,7 +1659,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C14" t="s">
         <v>150</v>
       </c>
@@ -1633,7 +1667,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>151</v>
       </c>
@@ -1641,7 +1675,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
         <v>152</v>
       </c>
@@ -1649,7 +1683,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
         <v>153</v>
       </c>
@@ -1657,7 +1691,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" t="s">
         <v>154</v>
       </c>
@@ -1665,7 +1699,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
         <v>155</v>
       </c>
@@ -1673,7 +1707,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>156</v>
       </c>
@@ -1681,7 +1715,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" t="s">
         <v>157</v>
       </c>
@@ -1689,7 +1723,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" t="s">
         <v>158</v>
       </c>
@@ -1697,7 +1731,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>159</v>
       </c>
@@ -1705,7 +1739,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>160</v>
       </c>
@@ -1713,7 +1747,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" t="s">
         <v>161</v>
       </c>
@@ -1721,7 +1755,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>162</v>
       </c>
@@ -1729,427 +1763,427 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D27" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D29" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D30" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D42" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D44" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D47" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D48" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D49" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D50" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D51" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D52" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D53" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D54" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D55" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D56" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D57" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D58" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D59" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D60" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D61" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D64" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D65" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D66" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D67" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D68" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D69" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D70" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D71" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D72" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D73" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D74" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D75" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D76" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D77" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D78" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D79" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D80" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D81" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="82" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D83" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="84" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="85" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D86" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="87" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D87" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="88" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D88" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="89" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D89" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="90" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D90" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="91" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D91" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="92" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D92" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D93" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="94" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D94" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="95" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D95" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="96" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D96" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D97" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D98" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D99" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="100" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D100" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D101" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="102" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D102" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="103" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D103" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="104" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D104" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="105" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D105" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="106" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D106" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="107" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D107" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="108" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D108" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D109" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="110" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D110" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="111" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D111" t="s">
         <v>136</v>
       </c>

</xml_diff>